<commit_message>
put these on the same scale
</commit_message>
<xml_diff>
--- a/visuals/pub_figures/Table2.xlsx
+++ b/visuals/pub_figures/Table2.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aminaly/Box Sync/heatwave_covid/visuals/pub_figures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1C96401C-1D50-C945-A2C1-FE187B328309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AB28950-A9BF-0A4C-825A-43BD53BA6DA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{DE66959F-4A02-374C-809F-DC0078C71063}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="24180" windowHeight="17500" activeTab="1" xr2:uid="{DE66959F-4A02-374C-809F-DC0078C71063}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Figure 1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>Model</t>
   </si>
@@ -66,13 +67,40 @@
   </si>
   <si>
     <t>Wet Bulb Temperature</t>
+  </si>
+  <si>
+    <t>Income Group</t>
+  </si>
+  <si>
+    <t>Minimum Income</t>
+  </si>
+  <si>
+    <t>Maximum Income</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Medium High</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>Medium Low</t>
+  </si>
+  <si>
+    <t>Low</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -87,6 +115,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -109,7 +150,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -117,10 +158,17 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="6" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -437,37 +485,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71A3FD5D-4BD4-5347-914B-236238AD2E65}">
-  <dimension ref="B2:F6"/>
+  <dimension ref="B2:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="15.83203125" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.1640625" customWidth="1"/>
+    <col min="6" max="6" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="2:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:6" ht="52" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
@@ -484,16 +533,19 @@
         <v>0.63070000000000004</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" t="s">
+    <row r="4" spans="2:6" ht="52" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="2:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="B5" s="3" t="s">
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="2:6" ht="52" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -505,12 +557,12 @@
       <c r="E5" s="1">
         <v>0</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="4">
         <v>0.63080000000000003</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="51" x14ac:dyDescent="0.2">
-      <c r="B6" s="3"/>
+    <row r="6" spans="2:6" ht="52" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="4"/>
       <c r="C6" s="1" t="s">
         <v>4</v>
       </c>
@@ -520,8 +572,9 @@
       <c r="E6" s="1">
         <v>0</v>
       </c>
-      <c r="F6" s="3"/>
-    </row>
+      <c r="F6" s="4"/>
+    </row>
+    <row r="10" spans="2:6" ht="35" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B5:B6"/>
@@ -529,4 +582,88 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C05A80E3-FEC6-9D4E-8D6F-14B8EBD44E8F}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="3" width="18" style="5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="5" customFormat="1" ht="38" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" s="5" customFormat="1" ht="38" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="7">
+        <v>129421</v>
+      </c>
+      <c r="C2" s="7">
+        <v>250001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" s="5" customFormat="1" ht="38" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="7">
+        <v>99803</v>
+      </c>
+      <c r="C3" s="7">
+        <v>129375</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="5" customFormat="1" ht="38" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="7">
+        <v>77000</v>
+      </c>
+      <c r="C4" s="7">
+        <v>99792</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" s="5" customFormat="1" ht="38" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="7">
+        <v>57446</v>
+      </c>
+      <c r="C5" s="7">
+        <v>76985</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" s="5" customFormat="1" ht="38" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="7">
+        <v>11406</v>
+      </c>
+      <c r="C6" s="7">
+        <v>57426</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>